<commit_message>
Uniform treatment of JSON subobjects.
</commit_message>
<xml_diff>
--- a/json.xlsx
+++ b/json.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\Source\Repos\xllquandl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\Source\Repos\xllinet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -345,15 +345,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H6"/>
+  <dimension ref="B2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -364,72 +363,78 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="str">
-        <f t="array" ref="B3:C5">_xll.JSON.GET(B2)</f>
-        <v>a</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
+      <c r="B3" s="1">
+        <f>_xll.JSON.PARSE(B2)</f>
+        <v>2.8662175186104709E-219</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
-        <v>b</v>
-      </c>
-      <c r="C4">
-        <v>5.4226421204045866E-227</v>
-      </c>
-      <c r="D4">
-        <f t="array" ref="D4:F4">_xll.RANGE.GET(C4)</f>
+        <f t="array" ref="B4:C6">_xll.JSON.GET(B3)</f>
+        <v>a</v>
+      </c>
+      <c r="C4" t="b">
         <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
-        <v>c</v>
+        <v>*b</v>
       </c>
       <c r="C5">
-        <v>5.4229641778430665E-227</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="array" ref="D5:E6">_xll.RANGE.GET(C5)</f>
-        <v>ca</v>
+        <v>1.4555692818784844E-200</v>
+      </c>
+      <c r="D5">
+        <f t="array" ref="D5:F5">_xll.JSON.GET(C5)</f>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>5.4076664495152733E-227</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <f t="array" ref="F5:H5">_xll.RANGE.GET(E5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <v>*c</v>
+      </c>
+      <c r="C6">
+        <v>1.4556091506582888E-200</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="array" ref="D6:E7">_xll.JSON.GET(C6)</f>
+        <v>*ca</v>
+      </c>
+      <c r="E6">
+        <v>6.4356433540120552E-201</v>
+      </c>
+      <c r="F6">
+        <f t="array" ref="F6:H6">_xll.JSON.GET(E6)</f>
         <v>4</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H6" t="str">
         <v>foo</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D6" t="str">
-        <v>cb</v>
-      </c>
-      <c r="E6">
-        <v>5.4104039377423521E-227</v>
-      </c>
-      <c r="F6" t="b">
-        <f t="array" ref="F6:H6">_xll.RANGE.GET(E6)</f>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <v>*cb</v>
+      </c>
+      <c r="E7">
+        <v>6.4357430259615661E-201</v>
+      </c>
+      <c r="F7" t="b">
+        <f t="array" ref="F7:H7">_xll.JSON.GET(E7)</f>
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>1.23</v>
       </c>
-      <c r="H6" t="e">
+      <c r="H7" t="e">
         <v>#NULL!</v>
       </c>
     </row>

</xml_diff>